<commit_message>
Commit on 2025-05-12 01:04:29
</commit_message>
<xml_diff>
--- a/I01_購物/03_Coupang/00_EXE/coupang_output.xlsx
+++ b/I01_購物/03_Coupang/00_EXE/coupang_output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
   <si>
     <t>id</t>
   </si>
@@ -40,124 +40,115 @@
     <t>DORO CAT 豆乳貓</t>
   </si>
   <si>
-    <t>DORO CAT 豆乳貓 混合豆腐礦物貓砂, 無味, 7L, 3袋</t>
-  </si>
-  <si>
-    <t>DORO CAT 豆乳貓 豆腐貓砂, 抹茶, 7L, 6袋</t>
-  </si>
-  <si>
-    <t>DORO CAT 豆乳貓 豆乳貓混合砂, 無味, 7L, 3包</t>
+    <t>DORO CAT 豆乳貓 活性碳與小蘇打雙重除臭顆粒低過敏極細豆腐貓砂, 無香, 7L, 2包</t>
+  </si>
+  <si>
+    <t>DORO CAT 豆乳貓 豆腐貓砂, 原味, 7L, 6袋</t>
+  </si>
+  <si>
+    <t>DORO CAT 豆乳貓 活性碳與小蘇打雙重除臭顆粒低過敏極細豆腐貓砂, 無香, 7L, 6包</t>
+  </si>
+  <si>
+    <t>DORO CAT 豆乳貓 豆腐貓砂, 無味, 7L, 1袋</t>
   </si>
   <si>
     <t>DORO CAT 豆乳貓 添加益生菌與小蘇打顆粒雙重除臭極細豆腐貓砂, 原味, 7L, 5包</t>
   </si>
   <si>
+    <t>DORO CAT 豆乳貓 活性碳與小蘇打雙重除臭顆粒低過敏極細豆腐貓砂, 無香, 7L, 1包</t>
+  </si>
+  <si>
     <t>DORO CAT 豆乳貓 添加酵素與小蘇打顆粒雙重消臭極細豆腐貓砂, 木質香, 7L, 4包</t>
   </si>
   <si>
-    <t>DORO CAT 豆乳貓 活性碳與小蘇打雙重除臭顆粒低過敏極細豆腐貓砂, 無香, 7L, 1包</t>
-  </si>
-  <si>
-    <t>DORO CAT 豆乳貓 豆腐貓砂, 無味, 7L, 1袋</t>
-  </si>
-  <si>
     <t>DOG CAT STAR 汪喵星球 益生菌消臭條型豆腐砂, 2.7kg, 6袋</t>
   </si>
   <si>
     <t>DORO CAT 豆乳貓 混合豆腐礦物貓砂, 無味, 7L, 4袋</t>
   </si>
   <si>
-    <t>DORO CAT 豆乳貓 添加益生菌與小蘇打顆粒雙重除臭極細豆腐貓砂, 原味, 7L, 3包</t>
-  </si>
-  <si>
-    <t>$416</t>
-  </si>
-  <si>
-    <t>$667</t>
-  </si>
-  <si>
-    <t>$384</t>
+    <t>DORO CAT 豆乳貓 豆腐貓砂, 抹茶, 7L, 1袋</t>
+  </si>
+  <si>
+    <t>$298</t>
+  </si>
+  <si>
+    <t>$675</t>
+  </si>
+  <si>
+    <t>$115</t>
   </si>
   <si>
     <t>$706</t>
   </si>
   <si>
-    <t>$581</t>
-  </si>
-  <si>
-    <t>$134</t>
-  </si>
-  <si>
-    <t>$115</t>
+    <t>$139</t>
+  </si>
+  <si>
+    <t>$597</t>
   </si>
   <si>
     <t>$857</t>
   </si>
   <si>
-    <t>$598</t>
-  </si>
-  <si>
-    <t>$396</t>
-  </si>
-  <si>
-    <t>($1.98/100ml)</t>
-  </si>
-  <si>
-    <t>($1.59/100ml)</t>
-  </si>
-  <si>
-    <t>($1.83/100ml)</t>
+    <t>$610</t>
+  </si>
+  <si>
+    <t>$114</t>
+  </si>
+  <si>
+    <t>($2.13/100ml)</t>
+  </si>
+  <si>
+    <t>($1.61/100ml)</t>
+  </si>
+  <si>
+    <t>($1.64/100ml)</t>
   </si>
   <si>
     <t>($2.02/100ml)</t>
   </si>
   <si>
-    <t>($2.08/100ml)</t>
-  </si>
-  <si>
-    <t>($1.92/100ml)</t>
-  </si>
-  <si>
-    <t>($1.64/100ml)</t>
+    <t>($1.99/100ml)</t>
   </si>
   <si>
     <t>($5.29/100g)</t>
   </si>
   <si>
-    <t>($2.14/100ml)</t>
-  </si>
-  <si>
-    <t>($1.89/100ml)</t>
-  </si>
-  <si>
-    <t>DORO CAT 豆乳貓 混合豆腐礦物貓砂, 無味, 7L, 3袋 特價 56折 $750 $416 ($1.98/100ml) 7折 優惠券 明天 5/12 (一) 預計送達 免運 滿 $490 ( 65 )</t>
-  </si>
-  <si>
-    <t>DORO CAT 豆乳貓 豆腐貓砂, 抹茶, 7L, 6袋 特價 45折 $1,500 $667 ($1.59/100ml) 7折 優惠券 明天 5/12 (一) 預計送達 免運 ( 489 )</t>
-  </si>
-  <si>
-    <t>DORO CAT 豆乳貓 豆乳貓混合砂, 無味, 7L, 3包 特價 52折 $750 $384 ($1.83/100ml) 7折 優惠券 明天 5/12 (一) 預計送達 免運 滿 $490 ( 1 )</t>
-  </si>
-  <si>
-    <t>DORO CAT 豆乳貓 添加益生菌與小蘇打顆粒雙重除臭極細豆腐貓砂, 原味, 7L, 5包 特價 57折 $1,250 $706 ($2.02/100ml) 7折 優惠券 明天 5/12 (一) 預計送達 免運 ( 90 )</t>
-  </si>
-  <si>
-    <t>DORO CAT 豆乳貓 添加酵素與小蘇打顆粒雙重消臭極細豆腐貓砂, 木質香, 7L, 4包 特價 59折 $1,000 $581 ($2.08/100ml) 7折 優惠券 明天 5/12 (一) 預計送達 免運 ( 50 )</t>
-  </si>
-  <si>
-    <t>DORO CAT 豆乳貓 活性碳與小蘇打雙重除臭顆粒低過敏極細豆腐貓砂, 無香, 7L, 1包 特價 54折 $250 $134 ($1.92/100ml) 7折 優惠券 明天 5/12 (一) 預計送達 免運 滿 $490 ( 52 )</t>
-  </si>
-  <si>
-    <t>DORO CAT 豆乳貓 豆腐貓砂, 無味, 7L, 1袋 特價 46折 $250 $115 ($1.64/100ml) 7折 優惠券 明天 5/12 (一) 預計送達 免運 滿 $490 ( 489 )</t>
-  </si>
-  <si>
-    <t>DOG CAT STAR 汪喵星球 益生菌消臭條型豆腐砂, 2.7kg, 6袋 特價 41折 $2,100 $857 ($5.29/100g) 7折 優惠券 明天 5/12 (一) 預計送達 免運 ( 2,633 )</t>
-  </si>
-  <si>
-    <t>DORO CAT 豆乳貓 混合豆腐礦物貓砂, 無味, 7L, 4袋 特價 6折 $1,000 $598 ($2.14/100ml) 7折 優惠券 明天 5/12 (一) 預計送達 免運 ( 65 )</t>
-  </si>
-  <si>
-    <t>DORO CAT 豆乳貓 添加益生菌與小蘇打顆粒雙重除臭極細豆腐貓砂, 原味, 7L, 3包 特價 53折 $750 $396 ($1.89/100ml) 7折 優惠券 明天 5/12 (一) 預計送達 免運 滿 $490 ( 90 )</t>
+    <t>($2.18/100ml)</t>
+  </si>
+  <si>
+    <t>($1.63/100ml)</t>
+  </si>
+  <si>
+    <t>DORO CAT 豆乳貓 活性碳與小蘇打雙重除臭顆粒低過敏極細豆腐貓砂, 無香, 7L, 2包 特價 6折 $500 $298 ($2.13/100ml) 7折 優惠券 缺貨 免運 滿 $490 ( 52 )</t>
+  </si>
+  <si>
+    <t>DORO CAT 豆乳貓 豆腐貓砂, 原味, 7L, 6袋 特價 45折 $1,500 $675 ($1.61/100ml) 7折 優惠券 缺貨 免運 ( 489 )</t>
+  </si>
+  <si>
+    <t>DORO CAT 豆乳貓 活性碳與小蘇打雙重除臭顆粒低過敏極細豆腐貓砂, 無香, 7L, 6包 特價 45折 $1,500 $675 ($1.61/100ml) 7折 優惠券 缺貨 免運 ( 52 )</t>
+  </si>
+  <si>
+    <t>DORO CAT 豆乳貓 豆腐貓砂, 無味, 7L, 1袋 特價 46折 $250 $115 ($1.64/100ml) 7折 優惠券 明天 5/13 (二) 預計送達 免運 滿 $490 ( 489 )</t>
+  </si>
+  <si>
+    <t>DORO CAT 豆乳貓 添加益生菌與小蘇打顆粒雙重除臭極細豆腐貓砂, 原味, 7L, 5包 特價 57折 $1,250 $706 ($2.02/100ml) 7折 優惠券 明天 5/13 (二) 預計送達 免運 ( 90 )</t>
+  </si>
+  <si>
+    <t>DORO CAT 豆乳貓 活性碳與小蘇打雙重除臭顆粒低過敏極細豆腐貓砂, 無香, 7L, 1包 特價 56折 $250 $139 ($1.99/100ml) 7折 優惠券 明天 5/13 (二) 預計送達 免運 滿 $490 ( 52 )</t>
+  </si>
+  <si>
+    <t>DORO CAT 豆乳貓 添加酵素與小蘇打顆粒雙重消臭極細豆腐貓砂, 木質香, 7L, 4包 特價 6折 $1,000 $597 ($2.13/100ml) 7折 優惠券 明天 5/13 (二) 預計送達 免運 ( 50 )</t>
+  </si>
+  <si>
+    <t>DOG CAT STAR 汪喵星球 益生菌消臭條型豆腐砂, 2.7kg, 6袋 特價 41折 $2,100 $857 ($5.29/100g) 7折 優惠券 明天 5/13 (二) 預計送達 免運 ( 2,633 )</t>
+  </si>
+  <si>
+    <t>DORO CAT 豆乳貓 混合豆腐礦物貓砂, 無味, 7L, 4袋 特價 61折 $1,000 $610 ($2.18/100ml) 7折 優惠券 明天 5/13 (二) 預計送達 免運 ( 65 )</t>
+  </si>
+  <si>
+    <t>DORO CAT 豆乳貓 豆腐貓砂, 抹茶, 7L, 1袋 特價 46折 $250 $114 ($1.63/100ml) 7折 優惠券 明天 5/13 (二) 預計送達 免運 滿 $490 ( 489 )</t>
   </si>
 </sst>
 </file>
@@ -550,7 +541,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -562,18 +553,18 @@
         <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G2" s="2">
-        <v>45788.87263888889</v>
+        <v>45789.03155092592</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -585,18 +576,18 @@
         <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G3" s="2">
-        <v>45788.87263888889</v>
+        <v>45789.03155092592</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4">
-        <v>28</v>
+        <v>88</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -605,21 +596,21 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G4" s="2">
-        <v>45788.87263888889</v>
+        <v>45789.03155092592</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5">
-        <v>27</v>
+        <v>87</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -628,21 +619,21 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G5" s="2">
-        <v>45788.87263888889</v>
+        <v>45789.03155092592</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -651,21 +642,21 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G6" s="2">
-        <v>45788.87263888889</v>
+        <v>45789.03155092592</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -674,21 +665,21 @@
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G7" s="2">
-        <v>45788.87263888889</v>
+        <v>45789.03155092592</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8">
-        <v>24</v>
+        <v>84</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -697,21 +688,21 @@
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G8" s="2">
-        <v>45788.87263888889</v>
+        <v>45789.03155092592</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -720,21 +711,21 @@
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G9" s="2">
-        <v>45788.87263888889</v>
+        <v>45789.03155092592</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -743,21 +734,21 @@
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G10" s="2">
-        <v>45788.87263888889</v>
+        <v>45789.03155092592</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -766,16 +757,16 @@
         <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G11" s="2">
-        <v>45788.87263888889</v>
+        <v>45789.03155092592</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit on 2025-05-16 23:45:47
</commit_message>
<xml_diff>
--- a/I01_購物/03_Coupang/00_EXE/coupang_output.xlsx
+++ b/I01_購物/03_Coupang/00_EXE/coupang_output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="84">
   <si>
     <t>id</t>
   </si>
@@ -37,118 +37,235 @@
     <t>timestamp</t>
   </si>
   <si>
-    <t>DORO CAT 豆乳貓</t>
-  </si>
-  <si>
-    <t>DORO CAT 豆乳貓 活性碳與小蘇打雙重除臭顆粒低過敏極細豆腐貓砂, 無香, 7L, 2包</t>
-  </si>
-  <si>
-    <t>DORO CAT 豆乳貓 豆腐貓砂, 原味, 7L, 6袋</t>
-  </si>
-  <si>
-    <t>DORO CAT 豆乳貓 活性碳與小蘇打雙重除臭顆粒低過敏極細豆腐貓砂, 無香, 7L, 6包</t>
-  </si>
-  <si>
-    <t>DORO CAT 豆乳貓 豆腐貓砂, 無味, 7L, 1袋</t>
-  </si>
-  <si>
-    <t>DORO CAT 豆乳貓 添加益生菌與小蘇打顆粒雙重除臭極細豆腐貓砂, 原味, 7L, 5包</t>
-  </si>
-  <si>
-    <t>DORO CAT 豆乳貓 活性碳與小蘇打雙重除臭顆粒低過敏極細豆腐貓砂, 無香, 7L, 1包</t>
-  </si>
-  <si>
-    <t>DORO CAT 豆乳貓 添加酵素與小蘇打顆粒雙重消臭極細豆腐貓砂, 木質香, 7L, 4包</t>
-  </si>
-  <si>
-    <t>DOG CAT STAR 汪喵星球 益生菌消臭條型豆腐砂, 2.7kg, 6袋</t>
-  </si>
-  <si>
-    <t>DORO CAT 豆乳貓 混合豆腐礦物貓砂, 無味, 7L, 4袋</t>
-  </si>
-  <si>
-    <t>DORO CAT 豆乳貓 豆腐貓砂, 抹茶, 7L, 1袋</t>
-  </si>
-  <si>
-    <t>$298</t>
-  </si>
-  <si>
-    <t>$675</t>
-  </si>
-  <si>
-    <t>$115</t>
-  </si>
-  <si>
-    <t>$706</t>
-  </si>
-  <si>
-    <t>$139</t>
-  </si>
-  <si>
-    <t>$597</t>
-  </si>
-  <si>
-    <t>$857</t>
-  </si>
-  <si>
-    <t>$610</t>
-  </si>
-  <si>
-    <t>$114</t>
-  </si>
-  <si>
-    <t>($2.13/100ml)</t>
-  </si>
-  <si>
-    <t>($1.61/100ml)</t>
-  </si>
-  <si>
-    <t>($1.64/100ml)</t>
-  </si>
-  <si>
-    <t>($2.02/100ml)</t>
-  </si>
-  <si>
-    <t>($1.99/100ml)</t>
-  </si>
-  <si>
-    <t>($5.29/100g)</t>
-  </si>
-  <si>
-    <t>($2.18/100ml)</t>
-  </si>
-  <si>
-    <t>($1.63/100ml)</t>
-  </si>
-  <si>
-    <t>DORO CAT 豆乳貓 活性碳與小蘇打雙重除臭顆粒低過敏極細豆腐貓砂, 無香, 7L, 2包 特價 6折 $500 $298 ($2.13/100ml) 7折 優惠券 缺貨 免運 滿 $490 ( 52 )</t>
-  </si>
-  <si>
-    <t>DORO CAT 豆乳貓 豆腐貓砂, 原味, 7L, 6袋 特價 45折 $1,500 $675 ($1.61/100ml) 7折 優惠券 缺貨 免運 ( 489 )</t>
-  </si>
-  <si>
-    <t>DORO CAT 豆乳貓 活性碳與小蘇打雙重除臭顆粒低過敏極細豆腐貓砂, 無香, 7L, 6包 特價 45折 $1,500 $675 ($1.61/100ml) 7折 優惠券 缺貨 免運 ( 52 )</t>
-  </si>
-  <si>
-    <t>DORO CAT 豆乳貓 豆腐貓砂, 無味, 7L, 1袋 特價 46折 $250 $115 ($1.64/100ml) 7折 優惠券 明天 5/13 (二) 預計送達 免運 滿 $490 ( 489 )</t>
-  </si>
-  <si>
-    <t>DORO CAT 豆乳貓 添加益生菌與小蘇打顆粒雙重除臭極細豆腐貓砂, 原味, 7L, 5包 特價 57折 $1,250 $706 ($2.02/100ml) 7折 優惠券 明天 5/13 (二) 預計送達 免運 ( 90 )</t>
-  </si>
-  <si>
-    <t>DORO CAT 豆乳貓 活性碳與小蘇打雙重除臭顆粒低過敏極細豆腐貓砂, 無香, 7L, 1包 特價 56折 $250 $139 ($1.99/100ml) 7折 優惠券 明天 5/13 (二) 預計送達 免運 滿 $490 ( 52 )</t>
-  </si>
-  <si>
-    <t>DORO CAT 豆乳貓 添加酵素與小蘇打顆粒雙重消臭極細豆腐貓砂, 木質香, 7L, 4包 特價 6折 $1,000 $597 ($2.13/100ml) 7折 優惠券 明天 5/13 (二) 預計送達 免運 ( 50 )</t>
-  </si>
-  <si>
-    <t>DOG CAT STAR 汪喵星球 益生菌消臭條型豆腐砂, 2.7kg, 6袋 特價 41折 $2,100 $857 ($5.29/100g) 7折 優惠券 明天 5/13 (二) 預計送達 免運 ( 2,633 )</t>
-  </si>
-  <si>
-    <t>DORO CAT 豆乳貓 混合豆腐礦物貓砂, 無味, 7L, 4袋 特價 61折 $1,000 $610 ($2.18/100ml) 7折 優惠券 明天 5/13 (二) 預計送達 免運 ( 65 )</t>
-  </si>
-  <si>
-    <t>DORO CAT 豆乳貓 豆腐貓砂, 抹茶, 7L, 1袋 特價 46折 $250 $114 ($1.63/100ml) 7折 優惠券 明天 5/13 (二) 預計送達 免運 滿 $490 ( 489 )</t>
+    <t>味丹 氣泡水</t>
+  </si>
+  <si>
+    <t>多喝水 氣泡水, 1.25L, 60瓶</t>
+  </si>
+  <si>
+    <t>Cloop 零卡氣泡飲 柚子口味, 6罐, 500ml</t>
+  </si>
+  <si>
+    <t>味丹 究.選 SUAN 草莓紅茶氣泡飲, 540ml, 72瓶</t>
+  </si>
+  <si>
+    <t>味丹 究‧選 SUÁN蜜桃紅茶氣泡飲, 540ml, 72瓶</t>
+  </si>
+  <si>
+    <t>DyDo Vida氣泡飲 青蘋果味, 325ml, 5罐</t>
+  </si>
+  <si>
+    <t>OOHA 氣泡飲 水蜜桃烏龍茶, 500ml, 24瓶</t>
+  </si>
+  <si>
+    <t>多喝水 氣泡水, 1.25L, 48瓶</t>
+  </si>
+  <si>
+    <t>味丹 七喜 汽水, 330ml, 24罐</t>
+  </si>
+  <si>
+    <t>TREE TOP 樹頂 蔓越莓氣泡飲, 320ml, 6罐</t>
+  </si>
+  <si>
+    <t>味丹 MORE+維他命氣泡水 乳酸風味, 560ml, 72瓶</t>
+  </si>
+  <si>
+    <t>OOHA 氣泡飲 水蜜桃烏龍茶 迷你罐, 200ml, 24罐</t>
+  </si>
+  <si>
+    <t>Tamsaa 無標籤氣泡水, 500ml, 20瓶</t>
+  </si>
+  <si>
+    <t>多喝水 氣泡水, 1.25L, 36瓶</t>
+  </si>
+  <si>
+    <t>DyDo Vida氣泡飲 青蘋果味, 325ml, 4罐</t>
+  </si>
+  <si>
+    <t>味丹 多喝水 MORE 原味氣泡水, 1.25L, 36瓶</t>
+  </si>
+  <si>
+    <t>味丹 究.選 SUAN 草莓紅茶氣泡飲, 540ml, 48瓶</t>
+  </si>
+  <si>
+    <t>TAISUN 泰山 Cheers EX 強氣泡水, 500ml, 24瓶</t>
+  </si>
+  <si>
+    <t>味丹 MORE氣泡水 蜜桃風味, 560ml, 72瓶</t>
+  </si>
+  <si>
+    <t>多喝水 氣泡水, 1.25L, 12瓶</t>
+  </si>
+  <si>
+    <t>味丹 多喝水 MORE 原味氣泡水, 1.25L, 24瓶</t>
+  </si>
+  <si>
+    <t>$1,991</t>
+  </si>
+  <si>
+    <t>$150</t>
+  </si>
+  <si>
+    <t>$1,097</t>
+  </si>
+  <si>
+    <t>$1,352</t>
+  </si>
+  <si>
+    <t>$125</t>
+  </si>
+  <si>
+    <t>$314</t>
+  </si>
+  <si>
+    <t>$1,573</t>
+  </si>
+  <si>
+    <t>$215</t>
+  </si>
+  <si>
+    <t>$132</t>
+  </si>
+  <si>
+    <t>$1,587</t>
+  </si>
+  <si>
+    <t>$206</t>
+  </si>
+  <si>
+    <t>$272</t>
+  </si>
+  <si>
+    <t>$1,154</t>
+  </si>
+  <si>
+    <t>$100</t>
+  </si>
+  <si>
+    <t>$1,195</t>
+  </si>
+  <si>
+    <t>$714</t>
+  </si>
+  <si>
+    <t>$299</t>
+  </si>
+  <si>
+    <t>$1,061</t>
+  </si>
+  <si>
+    <t>$318</t>
+  </si>
+  <si>
+    <t>$763</t>
+  </si>
+  <si>
+    <t>($2.66/100ml)</t>
+  </si>
+  <si>
+    <t>($5.00/100ml)</t>
+  </si>
+  <si>
+    <t>($2.82/100ml)</t>
+  </si>
+  <si>
+    <t>($3.48/100ml)</t>
+  </si>
+  <si>
+    <t>($7.69/100ml)</t>
+  </si>
+  <si>
+    <t>($2.62/100ml)</t>
+  </si>
+  <si>
+    <t>($2.72/100ml)</t>
+  </si>
+  <si>
+    <t>($6.88/100ml)</t>
+  </si>
+  <si>
+    <t>($3.94/100ml)</t>
+  </si>
+  <si>
+    <t>($4.29/100ml)</t>
+  </si>
+  <si>
+    <t>($2.57/100ml)</t>
+  </si>
+  <si>
+    <t>($2.76/100ml)</t>
+  </si>
+  <si>
+    <t>($2.49/100ml)</t>
+  </si>
+  <si>
+    <t>($2.63/100ml)</t>
+  </si>
+  <si>
+    <t>($2.12/100ml)</t>
+  </si>
+  <si>
+    <t>($2.54/100ml)</t>
+  </si>
+  <si>
+    <t>多喝水 氣泡水, 1.25L, 60瓶 特價 8折 $2,520 $1,991 ($2.66/100ml) 7折 優惠券 缺貨 免運 ( 919 )</t>
+  </si>
+  <si>
+    <t>Cloop 零卡氣泡飲 柚子口味, 6罐, 500ml 特價 43折 $352 $150 ($5.00/100ml) 5/26 預計送達 免運 滿 $690 ( 196 )</t>
+  </si>
+  <si>
+    <t>味丹 究.選 SUAN 草莓紅茶氣泡飲, 540ml, 72瓶 特價 74折 $1,497 $1,097 ($2.82/100ml) 7折 優惠券 5/19 星期一 預計送達 免運 ( 22 )</t>
+  </si>
+  <si>
+    <t>味丹 究‧選 SUÁN蜜桃紅茶氣泡飲, 540ml, 72瓶 特價 65折 $2,088 $1,352 ($3.48/100ml) 7折 優惠券 5/19 星期一 預計送達 免運 ( 144 )</t>
+  </si>
+  <si>
+    <t>DyDo Vida氣泡飲 青蘋果味, 325ml, 5罐 特價 65折 $195 $125 ($7.69/100ml) 明天 5/17 (六) 預計送達 免運 滿 $490 ( 76 ) 額外優惠券</t>
+  </si>
+  <si>
+    <t>OOHA 氣泡飲 水蜜桃烏龍茶, 500ml, 24瓶 特價 38折 $840 $314 ($2.62/100ml) 7折 優惠券 明天 5/17 (六) 預計送達 免運 滿 $490 ( 1,125 )</t>
+  </si>
+  <si>
+    <t>多喝水 氣泡水, 1.25L, 48瓶 特價 79折 $2,016 $1,573 ($2.62/100ml) 7折 優惠券 明天 5/17 (六) 預計送達 免運 ( 919 )</t>
+  </si>
+  <si>
+    <t>味丹 七喜 汽水, 330ml, 24罐 特價 36折 $600 $215 ($2.72/100ml) 7折 優惠券 明天 5/17 (六) 預計送達 免運 滿 $490 ( 566 )</t>
+  </si>
+  <si>
+    <t>TREE TOP 樹頂 蔓越莓氣泡飲, 320ml, 6罐 $132 ($6.88/100ml) 明天 5/17 (六) 預計送達 免運 滿 $490 ( 6 ) 額外優惠券</t>
+  </si>
+  <si>
+    <t>味丹 MORE+維他命氣泡水 乳酸風味, 560ml, 72瓶 $1,587 ($3.94/100ml) 明天 5/17 (六) 預計送達 免運 ( 5 ) 額外優惠券</t>
+  </si>
+  <si>
+    <t>OOHA 氣泡飲 水蜜桃烏龍茶 迷你罐, 200ml, 24罐 特價 7折 $295 $206 ($4.29/100ml) 7折 優惠券 明天 5/17 (六) 預計送達 免運 滿 $490 ( 5 )</t>
+  </si>
+  <si>
+    <t>Tamsaa 無標籤氣泡水, 500ml, 20瓶 $272 ($2.72/100ml) 明天 5/17 (六) 預計送達 免運 滿 $490 額外優惠券</t>
+  </si>
+  <si>
+    <t>多喝水 氣泡水, 1.25L, 36瓶 特價 77折 $1,512 $1,154 ($2.57/100ml) 7折 優惠券 明天 5/17 (六) 預計送達 免運 ( 919 )</t>
+  </si>
+  <si>
+    <t>DyDo Vida氣泡飲 青蘋果味, 325ml, 4罐 特價 65折 $156 $100 ($7.69/100ml) 明天 5/17 (六) 預計送達 免運 滿 $490 ( 76 ) 額外優惠券</t>
+  </si>
+  <si>
+    <t>味丹 多喝水 MORE 原味氣泡水, 1.25L, 36瓶 特價 8折 $1,512 $1,195 ($2.66/100ml) 7折 優惠券 明天 5/17 (六) 預計送達 免運 ( 326 )</t>
+  </si>
+  <si>
+    <t>味丹 究.選 SUAN 草莓紅茶氣泡飲, 540ml, 48瓶 特價 71折 $1,018 $714 ($2.76/100ml) 7折 優惠券 明天 5/17 (六) 預計送達 免運 ( 22 )</t>
+  </si>
+  <si>
+    <t>TAISUN 泰山 Cheers EX 強氣泡水, 500ml, 24瓶 特價 43折 $696 $299 ($2.49/100ml) 7折 優惠券 明天 5/17 (六) 預計送達 免運 滿 $490 ( 6,415 )</t>
+  </si>
+  <si>
+    <t>味丹 MORE氣泡水 蜜桃風味, 560ml, 72瓶 特價 57折 $1,872 $1,061 ($2.63/100ml) 7折 優惠券 明天 5/17 (六) 預計送達 免運 ( 722 )</t>
+  </si>
+  <si>
+    <t>多喝水 氣泡水, 1.25L, 12瓶 特價 64折 $504 $318 ($2.12/100ml) 7折 優惠券 明天 5/17 (六) 預計送達 免運 滿 $490 ( 919 )</t>
+  </si>
+  <si>
+    <t>味丹 多喝水 MORE 原味氣泡水, 1.25L, 24瓶 特價 76折 $1,008 $763 ($2.54/100ml) 7折 優惠券 明天 5/17 (六) 預計送達 免運 ( 326 )</t>
   </si>
 </sst>
 </file>
@@ -510,7 +627,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -541,7 +658,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2">
-        <v>90</v>
+        <v>484</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -550,21 +667,21 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="G2" s="2">
-        <v>45789.03155092592</v>
+        <v>45793.96263888889</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3">
-        <v>89</v>
+        <v>483</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -573,21 +690,21 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="F3" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="G3" s="2">
-        <v>45789.03155092592</v>
+        <v>45793.96263888889</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4">
-        <v>88</v>
+        <v>482</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -596,21 +713,21 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="F4" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="G4" s="2">
-        <v>45789.03155092592</v>
+        <v>45793.96263888889</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5">
-        <v>87</v>
+        <v>481</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -619,21 +736,21 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="G5" s="2">
-        <v>45789.03155092592</v>
+        <v>45793.96263888889</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6">
-        <v>86</v>
+        <v>480</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -642,21 +759,21 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="F6" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="G6" s="2">
-        <v>45789.03155092592</v>
+        <v>45793.96263888889</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7">
-        <v>85</v>
+        <v>479</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -665,21 +782,21 @@
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="G7" s="2">
-        <v>45789.03155092592</v>
+        <v>45793.96263888889</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8">
-        <v>84</v>
+        <v>478</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -688,21 +805,21 @@
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="F8" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="G8" s="2">
-        <v>45789.03155092592</v>
+        <v>45793.96263888889</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9">
-        <v>83</v>
+        <v>477</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -711,21 +828,21 @@
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="F9" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="G9" s="2">
-        <v>45789.03155092592</v>
+        <v>45793.96263888889</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10">
-        <v>82</v>
+        <v>476</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -734,21 +851,21 @@
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="F10" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="G10" s="2">
-        <v>45789.03155092592</v>
+        <v>45793.96263888889</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11">
-        <v>81</v>
+        <v>475</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -757,16 +874,246 @@
         <v>17</v>
       </c>
       <c r="D11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" s="2">
+        <v>45793.96263888889</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <v>474</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" s="2">
+        <v>45793.96263888889</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>473</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" t="s">
+        <v>75</v>
+      </c>
+      <c r="G13" s="2">
+        <v>45793.96263888889</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>472</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" t="s">
+        <v>76</v>
+      </c>
+      <c r="G14" s="2">
+        <v>45793.96263888889</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>471</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" t="s">
+        <v>77</v>
+      </c>
+      <c r="G15" s="2">
+        <v>45793.96263888889</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>470</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" t="s">
+        <v>78</v>
+      </c>
+      <c r="G16" s="2">
+        <v>45793.96263888889</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>469</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" t="s">
+        <v>79</v>
+      </c>
+      <c r="G17" s="2">
+        <v>45793.96263888889</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>468</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" t="s">
+        <v>80</v>
+      </c>
+      <c r="G18" s="2">
+        <v>45793.96263888889</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19">
+        <v>467</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G19" s="2">
+        <v>45793.96263888889</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20">
+        <v>466</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" t="s">
         <v>26</v>
       </c>
-      <c r="E11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" t="s">
-        <v>44</v>
-      </c>
-      <c r="G11" s="2">
-        <v>45789.03155092592</v>
+      <c r="D20" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" t="s">
+        <v>82</v>
+      </c>
+      <c r="G20" s="2">
+        <v>45793.96263888889</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21">
+        <v>465</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" t="s">
+        <v>63</v>
+      </c>
+      <c r="F21" t="s">
+        <v>83</v>
+      </c>
+      <c r="G21" s="2">
+        <v>45793.96263888889</v>
       </c>
     </row>
   </sheetData>

</xml_diff>